<commit_message>
feat/context : Testing another design for ground truth
</commit_message>
<xml_diff>
--- a/test/data/motor-pair-scenarii.xlsx
+++ b/test/data/motor-pair-scenarii.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\work\fll\mock\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2014FCA-A3B0-4318-9897-0CA8029C7C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C148527-8EF7-420E-9F1A-359418E50375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{2DAD570C-CE07-46E9-83B9-6BC7F65D4A4D}"/>
   </bookViews>
@@ -41,10 +41,10 @@
     <t>time</t>
   </si>
   <si>
-    <t>left degrees</t>
+    <t>left_degrees</t>
   </si>
   <si>
-    <t>right degrees</t>
+    <t>right_degrees</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:C384"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>